<commit_message>
added bbc article classfier
</commit_message>
<xml_diff>
--- a/8.Text_Mining/Naive_Bayes_from_scratch.xlsx
+++ b/8.Text_Mining/Naive_Bayes_from_scratch.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paragpradhan/Documents/Data Science Course/DS-Intro/8.Text_Mining/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C95113C-5E0D-6A43-9A8D-E7A68001D70B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81334DAF-567D-A044-A82D-D980E77F6DD9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16080" xr2:uid="{EA76C76F-82A6-2E4D-914E-96F3EB9CCF2A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16000" windowHeight="10720" xr2:uid="{EA76C76F-82A6-2E4D-914E-96F3EB9CCF2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="39">
   <si>
     <t>Hi you have won lottery</t>
   </si>
@@ -137,6 +137,18 @@
   </si>
   <si>
     <t>Probability</t>
+  </si>
+  <si>
+    <t>tag = spam</t>
+  </si>
+  <si>
+    <t>tag = ham</t>
+  </si>
+  <si>
+    <t>P(C|spam)*P(you|spam)…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -145,9 +157,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -230,9 +242,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -551,9 +563,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -561,7 +573,7 @@
     <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -569,7 +581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17" thickBot="1">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -582,8 +594,11 @@
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" thickTop="1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -594,8 +609,11 @@
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -603,7 +621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -611,35 +629,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -649,60 +685,136 @@
       <c r="C13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <f>B14/$B$8</f>
+        <v>0</v>
+      </c>
       <c r="D14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>E14/$B$9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" ref="C15:C18" si="0">B15/$B$8</f>
+        <v>0.14285714285714285</v>
+      </c>
       <c r="D15" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15:F18" si="1">E15/$B$9</f>
+        <v>7.1428571428571425E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
       <c r="D16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2857142857142857</v>
+      </c>
       <c r="D17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="7"/>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" s="7">
+        <f>B18/5</f>
+        <v>0.4</v>
+      </c>
       <c r="D18" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <f>E18/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19" s="9">
+        <f>C14*C15*C16*C17*C18</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="9">
+        <f>F14*F15*F16*F17*F18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -710,7 +822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="17" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -718,13 +830,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
@@ -741,95 +853,128 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>16</v>
       </c>
-      <c r="C26" t="e">
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
         <f>(B26+1)/($B$8 + $B$10)</f>
-        <v>#DIV/0!</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D26" t="s">
         <v>27</v>
       </c>
-      <c r="F26" t="e">
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <f>(E26+1)/($B$9 + $B$10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.2258064516129031E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="C27" t="e">
-        <f t="shared" ref="C27:C29" si="0">(B27+1)/($B$8 + $B$10)</f>
-        <v>#DIV/0!</v>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <f t="shared" ref="C27:C29" si="2">(B27+1)/($B$8 + $B$10)</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D27" t="s">
         <v>28</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" t="e">
-        <f t="shared" ref="F27:F29" si="1">(E27+1)/($B$9 + $B$10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" ref="F27:F29" si="3">(E27+1)/($B$9 + $B$10)</f>
+        <v>6.4516129032258063E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="C28" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D28" t="s">
         <v>29</v>
       </c>
-      <c r="F28" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>19</v>
       </c>
-      <c r="C29" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
       </c>
       <c r="D29" t="s">
         <v>30</v>
       </c>
-      <c r="F29" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>3.2258064516129031E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="9"/>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" s="9">
+        <f>B30/5</f>
+        <v>0.4</v>
+      </c>
       <c r="D30" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30" s="6">
+        <f>E30/5</f>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="6" t="e">
+      <c r="C31" s="6">
         <f>C26*C27*C28*C29*C30</f>
-        <v>#DIV/0!</v>
+        <v>1.4467592592592593E-5</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
-      <c r="F31" s="6" t="e">
+      <c r="F31" s="6">
         <f>F26*F27*F28*F29*F30</f>
-        <v>#DIV/0!</v>
+        <v>1.2993748923955163E-6</v>
       </c>
     </row>
   </sheetData>
@@ -846,7 +991,7 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
@@ -854,7 +999,7 @@
     <col min="4" max="4" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -862,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17" thickBot="1">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -876,7 +1021,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17" thickTop="1">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -888,7 +1033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -896,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -904,7 +1049,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -912,12 +1057,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -925,7 +1070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -933,7 +1078,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -941,12 +1086,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -968,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -990,7 +1135,7 @@
         <v>7.1428571428571425E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1012,7 +1157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1034,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1050,7 +1195,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="6" t="s">
         <v>22</v>
       </c>
@@ -1058,7 +1203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="17" thickBot="1">
       <c r="A22" s="4" t="s">
         <v>24</v>
       </c>
@@ -1066,13 +1211,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="4"/>
       <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
@@ -1089,7 +1234,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -1111,7 +1256,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1133,7 +1278,7 @@
         <v>6.4516129032258063E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1155,7 +1300,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1177,7 +1322,7 @@
         <v>3.2258064516129031E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" s="6" t="s">
         <v>21</v>
       </c>
@@ -1195,7 +1340,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="C31" s="6">

</xml_diff>